<commit_message>
Validación en eliminar materia / Código de Materia con 7 caracteres
</commit_message>
<xml_diff>
--- a/storage/app/plantillaExcel/ImportarMaterias.xlsx
+++ b/storage/app/plantillaExcel/ImportarMaterias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Desktop\UES_2020\SIGEN\sigen\storage\app\plantillaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FA1800-0079-42E4-A296-B8CBA96F8E66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D260B7-761F-464A-9242-5E67C3033AE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7893E2E6-40A3-4D99-A8F0-2B5F5FDD557B}"/>
   </bookViews>
@@ -363,15 +363,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -382,38 +373,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,13 +732,13 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="44" style="17" customWidth="1"/>
+    <col min="2" max="2" width="44" style="14" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" style="8" customWidth="1"/>
     <col min="4" max="4" width="21" style="8" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="4" customWidth="1"/>
@@ -746,12 +746,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -761,35 +761,35 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="15"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
     </row>
@@ -808,8 +808,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="G8" s="6" t="s">
@@ -818,7 +818,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
-      <c r="B9" s="16"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="G9" s="6" t="s">
@@ -827,121 +827,121 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="B10" s="16"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
-      <c r="B11" s="16"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="H11" s="27"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
-      <c r="B12" s="16"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="16"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="16"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="16"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="16"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" s="16"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="16"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="16"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="16"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
-      <c r="B21" s="16"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="16"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
-      <c r="B23" s="16"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
-      <c r="B24" s="16"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
-      <c r="B25" s="16"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
-      <c r="B26" s="16"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
-      <c r="B27" s="16"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
-      <c r="B28" s="16"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="5hveHMhqEKyldm/dNP8RzSEelRdfZ518XpfhXP9naNzxOkpQL4VgMO9N22JN2P59azkzk5rZoAJ3+v0qR1PmyA==" saltValue="TKx1gMUL+SLulykHn9/YYg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="uf1VfXNZnF6eqdHoLcIlyU37/YSCpghVXd8YqCsYh3QhZ8nw2xNrpKPVTVkaK8XWnUoXvONgfFo5upE888mx7A==" saltValue="nMfsJam7V1dmIeb3YkxOsg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="A2:D5"/>
     <mergeCell ref="A1:D1"/>
@@ -954,9 +954,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="¡Dato erroneo!" error="Solo puede ingresar 'Si' o No'._x000a_" sqref="C8:C1048576" xr:uid="{C46CE0A8-1AB4-46A8-816B-6562EC076700}">
       <formula1>$G$8:$G$9</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="¡Longitud Invalida!" error="El código de la materia puede tener de uno a seis caracteres._x000a_" sqref="A8:A1048576" xr:uid="{FAB84EA5-B493-4FB6-92C3-53577F91C4D9}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="¡Longitud Invalida!" error="El código de la materia puede tener de uno a siete caracteres._x000a_" sqref="A8:A1048576" xr:uid="{9DF52A64-DA77-4633-8FE0-6872F6644F16}">
       <formula1>1</formula1>
-      <formula2>6</formula2>
+      <formula2>7</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>